<commit_message>
feat(final remarks): adds final touches and notes
</commit_message>
<xml_diff>
--- a/4- 3.B/Observations/counts.xlsx
+++ b/4- 3.B/Observations/counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mors\Documents\SIAT\Semester 1\IAT804 - Foundations of Research Design for Human-Centred Design of Interactive Technologies\HW\4- 3.B\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F207243D-2351-49F0-AB05-74DA461D86BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD34462-5EBF-4311-B3B0-818BDDCD68E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC0362A6-8B80-4DBB-9C97-88A15413F059}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,8 +505,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <f>SUM(C1:O1)</f>
-        <v>13</v>
+        <f>SUM(C1:N1)</f>
+        <v>12</v>
       </c>
       <c r="C1" s="5">
         <v>1</v>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:B10" si="0">SUM(C2:O2)</f>
+        <f>SUM(C2:N2)</f>
         <v>9</v>
       </c>
       <c r="C2" s="5">
@@ -589,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C3:N3)</f>
         <v>2</v>
       </c>
       <c r="C3" s="5">
@@ -604,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C4:N4)</f>
         <v>1</v>
       </c>
       <c r="C4" s="5">
@@ -616,7 +616,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C5:N5)</f>
         <v>1</v>
       </c>
       <c r="C5" s="5">
@@ -628,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C6:N6)</f>
         <v>1</v>
       </c>
       <c r="C6" s="5">
@@ -640,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C7:N7)</f>
         <v>9</v>
       </c>
       <c r="C7" s="5">
@@ -676,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C8:N8)</f>
         <v>0</v>
       </c>
     </row>
@@ -685,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C9:N9)</f>
         <v>2</v>
       </c>
       <c r="C9" s="5">
@@ -700,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C10:N10)</f>
         <v>9</v>
       </c>
       <c r="C10" s="5">

</xml_diff>